<commit_message>
Trunk, Upper and Lower extremity bones and joints' datas are added.
Co-Authored-By: CaglaPelin <118660952+CaglaPelin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ai/data/raw/Project_MovementSystem_EDatas.xlsx
+++ b/ai/data/raw/Project_MovementSystem_EDatas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="297">
   <si>
     <t>id</t>
   </si>
@@ -272,13 +272,657 @@
   </si>
   <si>
     <t>["2 adet Concha Nasalis Inferior vardır.", "Burun boşluğu dış yan duvarındaki 3 konkadan alttakini oluşturur."]</t>
+  </si>
+  <si>
+    <t>columna_vertebralis</t>
+  </si>
+  <si>
+    <t>Columna Vertebralis</t>
+  </si>
+  <si>
+    <t>Trunk</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; omurga kanalı; lordoz; kifoz; omurilik</t>
+  </si>
+  <si>
+    <t>Gövdenin yükünü taşıyan kemik kolondur. Uzunluğu erişkin bir erkekte yaklaşık 70 cm, kadında ise 60 cm’dir. Vücudun dorsal bölgesinde artkafa kemiğinin altından başlayıp pelvise kadar uzanır. Bu kemik kolonda her bir omur deliğinin üst üste gelmesiyle omurga kanalı (canalis vertebralis) oluşur. Omurgaya yandan bakıldığında dört eğrilik görülür. Bunlar, boyun ve bel bölgesinde lordoz, göğüs ve sakrum bölgesinde kifozdur. Omurgada 33 omur olmasına rağmen 26 kemik bulunur. Bu 26 kemik arasında 23 tane omurlar arası disk (discus intervertebralis) bulunur.</t>
+  </si>
+  <si>
+    <t>["Omurga kanalı içerisinde omurilik bulunur ve bu sayede omurga omuriliği korur.", "Omurga baş, boyun ve gövdenin ağırlığını taşır.", "Omurga başın ve gövdenin hareketlerini sağlar."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.58</t>
+  </si>
+  <si>
+    <t>vertebrae_cervicales</t>
+  </si>
+  <si>
+    <t>Vertebrae cervicales</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; vertebrae cervicales; omur; vertebra; boyun; atlas; axis; lordoz</t>
+  </si>
+  <si>
+    <t>7 adet boyun omuru bulunur ve C1-C7 sembolleri ile gösterilirler. C1 omura atlas, C2 omura axis adı verilir. Atlas üst tarafta foramen magnumu çevreleyecek şekilde artkafa kemiği, alt tarafta ise axisle eklem yapar.</t>
+  </si>
+  <si>
+    <t>["Doğal lordoz eğriliği oluştururlar.", "Servikal omurlar küçüktür.", "Atlas ile axis arasında disk yoktur.", "Atlas ile axis kafanın hareketini sağlar."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.59</t>
+  </si>
+  <si>
+    <t>vertebrae_thoracicae</t>
+  </si>
+  <si>
+    <t>Vertebrae thoracicae</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; vertebrae thoracicae; omur; vertebra; göğüs; kifoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 adet göğüs omuru bulunur ve T1-T12 sembolleri ile gösterilirler. Kaburgalarla eklem yaparlar. </t>
+  </si>
+  <si>
+    <t>["Doğal kifoz eğriliği oluştururlar.", "Hareketleri boyun omurlarına kıyasla daha sınırlıdır."]</t>
+  </si>
+  <si>
+    <t>vertebrae_lumbales</t>
+  </si>
+  <si>
+    <t>Vertebrae lumbales</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; vertebrae lumbales; omur; vertebra; bel; lordoz; büyük; sağlam</t>
+  </si>
+  <si>
+    <t>5 adet bel omuru bulunur ve L1-L5 sembolleri ile gösterilirler.</t>
+  </si>
+  <si>
+    <t>["Doğal lordoz eğriliği oluştururlar.", "Gövdesi en büyük ve en sağlam omurlar lumbal bölgededir.", "Vücut ağırlığının büyük kısmını taşırlar."]</t>
+  </si>
+  <si>
+    <t>vertebrae_sacrale</t>
+  </si>
+  <si>
+    <t>Vertebrae sacrale (os sacrum)</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; vertebrae sacrale; os sacrum; omur; vertebra; kuyruk sokumu; sağrı; promontorium; kifoz; kemik</t>
+  </si>
+  <si>
+    <t>5 adet sağrı omuru bulunur ve S1-S5 sembolleri ile gösterilirler. Bu bölgedeki omurlar yetişkinlerde kaynaşıp bir kemiğe dönüşür.</t>
+  </si>
+  <si>
+    <t>["Doğal kifoz eğriliği oluştururlar.", "Promontorium adı verilen çıkıntı S1'in gövdesinin üst kenarında bulunur.", "Vücudun ağırlık merkezi S2’nin 2-2,5 cm önüne denk gelir."]</t>
+  </si>
+  <si>
+    <t>vertebrae_coccygea</t>
+  </si>
+  <si>
+    <t>Vertebrae coccygea (os coccyge)</t>
+  </si>
+  <si>
+    <t>columna vertebralis; omurga; vertebrae coccygea; os coccyge; omur; vertebra; kuyruk; kemik</t>
+  </si>
+  <si>
+    <t>4 adet kuyruk omuru bulunur ve Co1-Co4 sembolleri ile gösterilirler. Bu bölgedeki omurlar yetişkinlerde kaynaşıp bir kemiğe dönüşür.</t>
+  </si>
+  <si>
+    <t>["S5 ile Co1 arasında disk yoktur."]</t>
+  </si>
+  <si>
+    <t>thoracic_cage</t>
+  </si>
+  <si>
+    <t>Göğüs kafesi</t>
+  </si>
+  <si>
+    <t>thoracic cage; göğüs kafesi; göğüs boşluğu; koruma</t>
+  </si>
+  <si>
+    <t>Önde göğüs tahtası kemiği (Os Sternum) ile 12 çift kaburgadan (Ossa Costae) oluşur. Arka bölümünde göğüs
+omurları bulunur. Göğüs kafesinin iç kısmına göğüs boşluğu denir. Bu boşlukta kalp ve akciğer gibi önemli organlar bulunur.</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.60</t>
+  </si>
+  <si>
+    <t>os_sternum</t>
+  </si>
+  <si>
+    <t>Os Sternum</t>
+  </si>
+  <si>
+    <t>thoracic cage; göğüs kafesi; os sternum; göğüs tahtası kemiği; manubrium sterni; sternum sapı; corpus sterni; sternum
+gövdesi; processus xiphoideus; hançersi çıkıntı</t>
+  </si>
+  <si>
+    <t>Üç kısımdan oluşur. Üstteki kısmına sternum sapı (manubrium sterni), ortadaki kısmına sternum
+gövdesi (corpus sterni) ve uç kısmına ise hançersi çıkıntı (processus xiphoideus) denir.</t>
+  </si>
+  <si>
+    <t>["Manubrium sterni hem köprücük kemiği (clavicula) hem de 1 ve 2’nci kaburga ile eklem yapar.", "Corpus sterni her iki tarafında bulunan 2 ve 7’nci kaburgalarla eklem yapar.", "Processus xiphoideus kaburgalarla eklem yapmaz."]</t>
+  </si>
+  <si>
+    <t>ossa_costae</t>
+  </si>
+  <si>
+    <t>Ossa Costae</t>
+  </si>
+  <si>
+    <t>thoracic cage; göğüs kafesi; ossa costae; kaburga; kosta; gerçek kaburga; yalancı kaburga; yüzen kaburga</t>
+  </si>
+  <si>
+    <t>Baş kısımları (caput costae) arkada göğüs omurlarıyla eklem yapar. Kaburgalar sternuma bağlanma özelliklerine göre iki gruba ayrılır. Sternumla doğrudan eklem yapan ilk 7 çift kaburgaya gerçek kaburga denir. Son 5 çift kaburgaya ise yalancı kaburga denir. Yalancı kaburgaların ilk 3 çiftinin (8, 9 ve 10’uncu) kıkırdakları önce kendi aralarında birleşip 7’nci kaburganın kıkırdağına katılır ve sternumla dolaylı eklem yapar. Son 2 çift yalancı kaburga (11 ve 12’nci) kasların içinde serbest olarak sonlanır ve yüzen kaburga olarak adlandırılır.</t>
+  </si>
+  <si>
+    <t>os_clavicula</t>
+  </si>
+  <si>
+    <t>Os Clavicula</t>
+  </si>
+  <si>
+    <t>Upper_Extremity</t>
+  </si>
+  <si>
+    <t>cingulum membri superioris; omuz; köprücük kemiği; köprü</t>
+  </si>
+  <si>
+    <t>Her iki omzun ön tarafında hem kürek kemiği hem de sternum ile eklem yapar. Vücutta en sık kırılan
+kemiktir. Omuzla göğüs arasında köprü görevi yapar. Kemikleşmeye ilk başlayan kemiktir.</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.61</t>
+  </si>
+  <si>
+    <t>os_scapula</t>
+  </si>
+  <si>
+    <t>Os Scapula</t>
+  </si>
+  <si>
+    <t>cingulum membri superioris; omuz; kürek kemiği; acromion; korakoid çıkıntı; processus coracoideus; glenoid çukur; cavitas glenoidalis</t>
+  </si>
+  <si>
+    <t>Her iki omzun arka bölgesinde T2-T7 arasında yer alır. Arkadan dış yana doğru uzanan çıkıntısına acromion denir. Acromion çıkıntısı köprücük kemiği ile eklem yapar. Üst dış yanda öne doğru uzanan ve bazı kasların tutunduğu gagaya benzer çıkıntısına korakoid çıkıntı (processus coracoideus) denir. Üst dış kenarında ise kol kemiğiyle eklem yapan glenoid çukur (cavitas glenoidalis) bulunur.</t>
+  </si>
+  <si>
+    <t>os_humerus</t>
+  </si>
+  <si>
+    <t>Os Humerus</t>
+  </si>
+  <si>
+    <t>brachium; kol; kol kemiği; uzun; caput humeri; humerus başı; trochlea humeri; humerus makarası; capitulum humeri; humerus başçığı</t>
+  </si>
+  <si>
+    <t>Omuz ve dirsek eklemi arasında bulunan kemiktir. Humerus başı (caput humeri), kürek kemiği ile eklem (omuz eklemi) yapar. Alt ucu iki ön kol kemiği ile eklem (dirsek eklemi) yapar. İç yandaki dirsek kemiği ile eklem yapan kısmına humerus makarası (trochlea humeri) ve dış yandaki döner kemikle eklem yapan kısmına humerus başçığı (capitulum humeri) denir.</t>
+  </si>
+  <si>
+    <t>["Üst ekstremitenin en uzun kemiğidir."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.62</t>
+  </si>
+  <si>
+    <t>os_ulna</t>
+  </si>
+  <si>
+    <t>Os Ulna</t>
+  </si>
+  <si>
+    <t>antebrachium; ön kol; dirsek kemiği; olecranon; dirsek çıkıntısı; caput ulnae; ulna başı; serçe parmak</t>
+  </si>
+  <si>
+    <t>Serçe parmak tarafındaki kemiktir. Humerus ile eklem yapan üst ucuna olecranon (dirsek çıkıntısı) denir. Ulna başı (caput ulnae) aşağıda olup bilek eklemine katılır.</t>
+  </si>
+  <si>
+    <t>os_radius</t>
+  </si>
+  <si>
+    <t>Os Radius</t>
+  </si>
+  <si>
+    <t>antebrachium; ön kol; döner kemik; caput radii; radius başı; başparmak</t>
+  </si>
+  <si>
+    <t>Başparmak tarafındaki kemiktir. Üstteki radius başı (caput radii) humerus ile eklem yapar. Anatomik duruşta ulna ile paraleldir. Öne uzatılan elin avuç içi aşağı çevrildiğinde bu kemik ulnanın üzerine doğru döner. Alt ucu bilek eklemine katılır.</t>
+  </si>
+  <si>
+    <t>ossa_carpi</t>
+  </si>
+  <si>
+    <t>Ossa Carpi</t>
+  </si>
+  <si>
+    <t>manus; el; bilek; el bileği</t>
+  </si>
+  <si>
+    <t>El bileğinde 4’erli iki sıra halinde 8 kısa kemik bulunur. Ön kol kemikleri ile el tarağı kemikleri arasında yer alır. Kaslar ve bağlarla birbirine sıkıca bağlandıkları için hareketleri kısıtlıdır.</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.63</t>
+  </si>
+  <si>
+    <t>ossa_metacarpi</t>
+  </si>
+  <si>
+    <t>Ossa Metacarpi</t>
+  </si>
+  <si>
+    <t>manus; el; tarak; el tarak</t>
+  </si>
+  <si>
+    <t>Avuç içi ve el sırtının iskeletini oluşturan 5 uzun kemiktir. El bileği kemikleri ile parmak kemikleri arasında bulunur.</t>
+  </si>
+  <si>
+    <t>ossa_digitorum_manus</t>
+  </si>
+  <si>
+    <t>Ossa Digitorum Manus (Phalanges)</t>
+  </si>
+  <si>
+    <t>manus; el; parmak; el parmak</t>
+  </si>
+  <si>
+    <t>Beş parmakta toplam 14 kemik bulunur. Kemik sayısı başparmakta 2 diğer parmaklarda 3’er tanedir.</t>
+  </si>
+  <si>
+    <t>os_coxa</t>
+  </si>
+  <si>
+    <t>Os Coxa</t>
+  </si>
+  <si>
+    <t>Lower_Extremity</t>
+  </si>
+  <si>
+    <t>alt ekstremite; kalça; pelvis; çift; düzensiz; acetabulum</t>
+  </si>
+  <si>
+    <t>Pelvisin yan duvarını oluşturan ve uyluk kemiği ile eklem yapan kalça kemiğidir.</t>
+  </si>
+  <si>
+    <t>["Dış yüzünde femur ile eklem yapan çanak şeklinde acetabulum bulunur.", "Sağ ve sol olmak üzere 2 adet os coxae vardır.", "Sakrum ile birlikte pelvis boşluğunu oluşturur.", "Üç kemiğin birleşmesiyle oluşur.", "15–16 yaşlarında kaynaşarak tek kemik haline gelir."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_ilium
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os Ilium
+</t>
+  </si>
+  <si>
+    <t>alt ekstremite; kalça; pelvis; üst; yassı; ilium</t>
+  </si>
+  <si>
+    <t>Os coxae’nin üst bölümünü oluşturan geniş kemiktir.</t>
+  </si>
+  <si>
+    <t>["Os coxae’nin en geniş parçasıdır.", "Pelvisin üst bölümünü oluşturur.", "Arkada sakrumdan başlayarak öne doğru geniş bir kavis çizer.", "Önde os pubis ile birleşir."]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_pubis
+</t>
+  </si>
+  <si>
+    <t>Os Pubis</t>
+  </si>
+  <si>
+    <t>alt ekstremite; kalça; pelvis; ön; pubis; eklem</t>
+  </si>
+  <si>
+    <t>Os coxae’nin ön bölümünü oluşturan kemiktir.</t>
+  </si>
+  <si>
+    <t>["Os coxae’nin ön bölümünü oluşturur.", "Karşılıklı iki çatı kemiği ön alt tarafta birbiriyle eklemleşir"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_ischii
+</t>
+  </si>
+  <si>
+    <t>Os Ischii</t>
+  </si>
+  <si>
+    <t>alt ekstremite; kalça; pelvis; alt; arka; ischii</t>
+  </si>
+  <si>
+    <t>Os coxae’nin alt-arka bölümünü oluşturan kemiktir.</t>
+  </si>
+  <si>
+    <t>["Oturur pozisyonda gövde ağırlığını taşır.", "Çatı kemiğiyle beraber foramen obturatumu oluşturur"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_femur
+</t>
+  </si>
+  <si>
+    <t>Os Femur</t>
+  </si>
+  <si>
+    <t>alt ekstremite; uyluk; uzun; çift; femur</t>
+  </si>
+  <si>
+    <t>İskeletin en büyük, en uzun ve en sağlam kemiğidir.</t>
+  </si>
+  <si>
+    <t>["Femur başı (caput femoris) kalça kemiğinin acetabulum çukuru ile eklem yapar.", "Alt ucunda kaval kemiği ile eklem yapan iki yumrusu (condylus) bulunur."]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_patella
+</t>
+  </si>
+  <si>
+    <t>Os Patella</t>
+  </si>
+  <si>
+    <t>alt ekstremite; uyluk; diz; susamsı; patella</t>
+  </si>
+  <si>
+    <t>Vücudun en büyük susamsı kemiğidir.</t>
+  </si>
+  <si>
+    <t>["Dört başlı femur kasının tendonu içine yerleşmiştir", "Femur ile eklem yaparak diz eklemine katılır."]</t>
+  </si>
+  <si>
+    <t>os_tibia</t>
+  </si>
+  <si>
+    <t>Os Tibia</t>
+  </si>
+  <si>
+    <t>alt ekstremite; baldır; iç; uzun; tibia</t>
+  </si>
+  <si>
+    <t>Baldır bölgesinin iç yanında bulunan büyük kemiktir.</t>
+  </si>
+  <si>
+    <t>["Tibia başı (caput tibia) yukarıda femur ile eklem yapar", "Alt ucu ayak bileği eklemine katılır.", "Dış yanında kamış kemikle eklem yapar."]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">os_fibula
+</t>
+  </si>
+  <si>
+    <t>Os Fibula</t>
+  </si>
+  <si>
+    <t>alt ekstremite; baldır; dış; ince; fibula</t>
+  </si>
+  <si>
+    <t>Baldır bölgesinde yer alan ince kemiktir.</t>
+  </si>
+  <si>
+    <t>["Diz eklemine katılmaz.", "Kemik başı tibia kemiğinin dış yanındaki yumru ile eklem yapar.", "Alt ucu ayak bileği eklemine katılır."]</t>
+  </si>
+  <si>
+    <t>ossa_tarsi</t>
+  </si>
+  <si>
+    <t>Ossa Tarsi</t>
+  </si>
+  <si>
+    <t>alt ekstremite; ayak; ayak bileği; kısa; tarsal</t>
+  </si>
+  <si>
+    <t>Ayak bileğinde yer alan kısa kemik grubudur.</t>
+  </si>
+  <si>
+    <t>["Ayak bileğinde iki sıra halinde dizilmiş 7 kısa kemik bulunur.", "Baldır kemikleri ile ayak tarak kemikleri arasında yer alır.", "Aşık kemiği (os talus), tibia ve fibula ile ayak bileği eklemini oluşturur.", "Ayak bileğindeki en büyük kemik topuk kemiğidir (os calcaneus)."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.65</t>
+  </si>
+  <si>
+    <t>ossa_metatarsi</t>
+  </si>
+  <si>
+    <t>Ossa Metatarsi</t>
+  </si>
+  <si>
+    <t>alt ekstremite; ayak; tarak; uzun; metatarsal</t>
+  </si>
+  <si>
+    <t>Ayak tabanı ve ayak sırtının iskeletini oluşturan kemik grubudur.</t>
+  </si>
+  <si>
+    <t>["5 uzun kemikten oluşur.", "Ayak bileği kemikleri ile ayak parmak kemikleri arasında yer alır."]</t>
+  </si>
+  <si>
+    <t>ossa_digitorum_pedis</t>
+  </si>
+  <si>
+    <t>Ossa Digitorum Pedis</t>
+  </si>
+  <si>
+    <t>alt ekstremite; ayak; parmak; falanks</t>
+  </si>
+  <si>
+    <t>Ayak parmaklarını oluşturan kemik grubudur.</t>
+  </si>
+  <si>
+    <t>["Başparmakta 2 parmak kemiği bulunur.", "Diğer parmaklarda 3’er tane parmak kemiği bulunur.", "Toplam 14 parmak kemiğinden oluşur."]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sutura
+</t>
+  </si>
+  <si>
+    <t>Joint</t>
+  </si>
+  <si>
+    <t>Sutura</t>
+  </si>
+  <si>
+    <t>Joints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eklem; oynamaz; fibroz; sutura
+</t>
+  </si>
+  <si>
+    <t>Kafa kemikleri arasında bulunan oynamaz, dikiş tarzı eklemdir.</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gomphosis
+</t>
+  </si>
+  <si>
+    <t>Gomphosis</t>
+  </si>
+  <si>
+    <t>eklem; oynamaz; fibroz; gomphosis</t>
+  </si>
+  <si>
+    <t>Diş kökü ile çene kemiği arasında bulunan oynamaz eklemdir.</t>
+  </si>
+  <si>
+    <t>syndesmosis</t>
+  </si>
+  <si>
+    <t>Syndesmosis</t>
+  </si>
+  <si>
+    <t>eklem; oynamaz; fibroz; syndesmosis</t>
+  </si>
+  <si>
+    <t>Kemik yüzlerinin birbirine ligamentlerle bağlandığı oynamaz eklemdir.</t>
+  </si>
+  <si>
+    <t>["Kemik yüzleri birbirine ligamentlerle sıkıca bağlanmıştır.", "Örnek: Ulna ile radius arasındaki eklem."]</t>
+  </si>
+  <si>
+    <t>synchondrosis</t>
+  </si>
+  <si>
+    <t>Synchondrosis</t>
+  </si>
+  <si>
+    <t>eklem; yarı oynar; synchondrosis; kartilaginoz; hiyalin kıkırdak; sternum; kosta; epifiz plak</t>
+  </si>
+  <si>
+    <t>Eklem yüzleri arasında hiyalin kıkırdak bulunan yarı oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Örnek: Kaburgalar ile sternum arasındaki eklemler.", "Örnek: Uzun kemiklerin epifiz plakları."]</t>
+  </si>
+  <si>
+    <t>symphysis</t>
+  </si>
+  <si>
+    <t>Symphysis</t>
+  </si>
+  <si>
+    <t>eklem; yarı oynar; kartilaginoz; fibroz kıkırdak; disk; pelvis; omur</t>
+  </si>
+  <si>
+    <t>Eklem yüzleri arasında fibroz kıkırdak yapısında disk bulunan yarı oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Örnek: Pubis kemikleri arasındaki eklem (symphysis pubis).", "Örnek: Omurlar arasındaki eklemler (symphysis intervertebralis)."]</t>
+  </si>
+  <si>
+    <t>art_temporomandibularis</t>
+  </si>
+  <si>
+    <t>Art. Temporomandibularis</t>
+  </si>
+  <si>
+    <t>eklem; oynar; temporomandibular; çene; kafa</t>
+  </si>
+  <si>
+    <t>Kafa bölgesinin tek oynar eklemidir.</t>
+  </si>
+  <si>
+    <t>["Temporal ve mandibular kemik arasında bulunur.", "Alt çeneyi dış yana, iç yana, öne ve arkaya doğru hareket ettirir.", "Alt çeneyi yukarı ve aşağı doğru hareket ettirir."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.70</t>
+  </si>
+  <si>
+    <t>art_atlantooccipitalis</t>
+  </si>
+  <si>
+    <t>Art. Atlantooccipitalis</t>
+  </si>
+  <si>
+    <t>eklem; oynar; atlantooccipital; atlas; oksipital</t>
+  </si>
+  <si>
+    <t>Oksipital kemik ile atlas arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Başa fleksiyon, ekstansiyon ve biraz da lateral fleksiyon yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_atlantoaxialis</t>
+  </si>
+  <si>
+    <t>Art. Atlantoaxialis</t>
+  </si>
+  <si>
+    <t>eklem; oynar; atlantoaxial; atlas; eksen</t>
+  </si>
+  <si>
+    <t>Atlas ile eksen arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Başa rotasyon hareketi yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_humeri</t>
+  </si>
+  <si>
+    <t>Art. Humeri</t>
+  </si>
+  <si>
+    <t>eklem; oynar; omuz; humerus; skapula</t>
+  </si>
+  <si>
+    <t>Humerus başı ile skapula kemiği arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Vücudun en fazla hareket yeteneğine sahip eklemidir.",  "Kola tüm hareketleri yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_cubiti</t>
+  </si>
+  <si>
+    <t>Art. Cubiti</t>
+  </si>
+  <si>
+    <t>eklem; oynar; dirsek; humerus; ulna; radius</t>
+  </si>
+  <si>
+    <t>Humerus, ulna ve radius kemikleri arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Üç ayrı eklemden oluşur.", "Hem fleksiyon ve ekstansiyon hem de pronasyon ve supinasyon yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_ radiocarpalis</t>
+  </si>
+  <si>
+    <t>Art. Radiocarpalis</t>
+  </si>
+  <si>
+    <t>eklem; oynar; el bileği; radius; karpal</t>
+  </si>
+  <si>
+    <t>Proksimaldeki üç karpal kemik ile radius kemiği arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Ulna kemiği bu ekleme girmez.", "El bileğine fleksiyon , ekstansiyon, abdüksiyon, addüksiyon, sirkümdüksiyon yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_coxae</t>
+  </si>
+  <si>
+    <t>Art. Coxae</t>
+  </si>
+  <si>
+    <t>eklem; oynar; kalça; acetabulum; femur</t>
+  </si>
+  <si>
+    <t>Kalça kemiğinin acetabulum çukuru ile femur başı arasındaki oynar eklemdir.</t>
+  </si>
+  <si>
+    <t>["Bacağa tüm hareketleri yaptırır."]</t>
+  </si>
+  <si>
+    <t>art_genus</t>
+  </si>
+  <si>
+    <t>Art. Genus</t>
+  </si>
+  <si>
+    <t>eklem; oynar; diz; femur; tibia; patella</t>
+  </si>
+  <si>
+    <t>Vücudun en büyük ve karmaşık eklemlerinden biridir.</t>
+  </si>
+  <si>
+    <t>["Femur, tibia ve patella kemikleri arasındadır.", "Fibula kemiği bu ekleme katılmaz.", "Eklem yüzleri arasında menisküsler vardır.", "Eklem ön yüzünde patella bulunur.", "Dize fleksiyon ve ekstansiyon yaptırır.", "Yarı fleksiyonda biraz iç ve dış rotasyon yaptırır."]</t>
+  </si>
+  <si>
+    <t>Ders kitabı s.71</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -289,6 +933,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,12 +953,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,6 +1708,1410 @@
         <v>52</v>
       </c>
     </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" ht="15.0" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>